<commit_message>
adding fsos and assortment
</commit_message>
<xml_diff>
--- a/Projects/CARLSBRGHK/Data/Template.xlsx
+++ b/Projects/CARLSBRGHK/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="kpis" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="38">
   <si>
     <t xml:space="preserve">kpi_name</t>
   </si>
@@ -167,7 +167,7 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -207,13 +207,19 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC5C2F5"/>
-        <bgColor rgb="FFC0C0C0"/>
+        <bgColor rgb="FF99CCFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF977D"/>
         <bgColor rgb="FFF69ABE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFC2E8FB"/>
       </patternFill>
     </fill>
   </fills>
@@ -258,7 +264,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -323,6 +329,10 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -352,7 +362,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -406,16 +416,16 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B3 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="110.826530612245"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="105.969387755102"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.50510204081633"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -551,24 +561,26 @@
   </sheetPr>
   <dimension ref="1:11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="58.3520408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="59.530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="7" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="7" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="7" width="29.0255102040816"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="7" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="7" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="17" min="15" style="7" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="7" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="7" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="51.4336734693878"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="60.2040816326531"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="7" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="7" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="7" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="7" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="7" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="7" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="17" min="15" style="7" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="7" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="7" width="9.85204081632653"/>
   </cols>
   <sheetData>
     <row r="1" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -632,14 +644,14 @@
       <c r="D2" s="13"/>
       <c r="E2" s="14"/>
       <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
+      <c r="G2" s="16"/>
       <c r="H2" s="12" t="s">
         <v>31</v>
       </c>
       <c r="I2" s="13"/>
       <c r="J2" s="14"/>
       <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
+      <c r="L2" s="16"/>
       <c r="M2" s="2" t="s">
         <v>30</v>
       </c>
@@ -1662,7 +1674,7 @@
       <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="17" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1676,14 +1688,14 @@
       </c>
       <c r="E3" s="14"/>
       <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
+      <c r="G3" s="16"/>
       <c r="H3" s="12" t="s">
         <v>31</v>
       </c>
       <c r="I3" s="13"/>
       <c r="J3" s="14"/>
       <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
+      <c r="L3" s="16"/>
       <c r="M3" s="2" t="s">
         <v>30</v>
       </c>
@@ -2706,7 +2718,7 @@
       <c r="AMJ3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="17" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -2720,12 +2732,12 @@
       </c>
       <c r="E4" s="14"/>
       <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
+      <c r="G4" s="16"/>
       <c r="H4" s="12"/>
       <c r="I4" s="13"/>
       <c r="J4" s="14"/>
       <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
+      <c r="L4" s="16"/>
       <c r="M4" s="2" t="s">
         <v>30</v>
       </c>
@@ -3748,7 +3760,7 @@
       <c r="AMJ4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="17" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -3764,12 +3776,12 @@
         <v>35</v>
       </c>
       <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
+      <c r="G5" s="16"/>
       <c r="H5" s="12"/>
       <c r="I5" s="13"/>
       <c r="J5" s="14"/>
       <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
+      <c r="L5" s="16"/>
       <c r="M5" s="2" t="s">
         <v>35</v>
       </c>
@@ -4792,7 +4804,7 @@
       <c r="AMJ5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="17" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -4810,12 +4822,12 @@
       <c r="F6" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="15"/>
+      <c r="G6" s="16"/>
       <c r="H6" s="12"/>
       <c r="I6" s="13"/>
       <c r="J6" s="14"/>
       <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
+      <c r="L6" s="16"/>
       <c r="M6" s="2" t="s">
         <v>36</v>
       </c>
@@ -5850,14 +5862,14 @@
       </c>
       <c r="E7" s="14"/>
       <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
+      <c r="G7" s="16"/>
       <c r="H7" s="12" t="s">
         <v>31</v>
       </c>
       <c r="I7" s="13"/>
       <c r="J7" s="14"/>
       <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
+      <c r="L7" s="16"/>
       <c r="M7" s="2" t="s">
         <v>30</v>
       </c>
@@ -5890,14 +5902,14 @@
         <v>34</v>
       </c>
       <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
+      <c r="G8" s="16"/>
       <c r="H8" s="12" t="s">
         <v>31</v>
       </c>
       <c r="I8" s="13"/>
       <c r="J8" s="14"/>
       <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
+      <c r="L8" s="16"/>
       <c r="M8" s="2" t="s">
         <v>30</v>
       </c>
@@ -6936,12 +6948,12 @@
         <v>34</v>
       </c>
       <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
+      <c r="G9" s="16"/>
       <c r="H9" s="12"/>
       <c r="I9" s="13"/>
       <c r="J9" s="14"/>
       <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
+      <c r="L9" s="16"/>
       <c r="M9" s="2" t="s">
         <v>30</v>
       </c>
@@ -7982,12 +7994,12 @@
       <c r="F10" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G10" s="15"/>
+      <c r="G10" s="16"/>
       <c r="H10" s="12"/>
       <c r="I10" s="13"/>
       <c r="J10" s="14"/>
       <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
+      <c r="L10" s="16"/>
       <c r="M10" s="2" t="s">
         <v>35</v>
       </c>
@@ -9028,12 +9040,14 @@
       <c r="F11" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G11" s="15"/>
+      <c r="G11" s="16" t="s">
+        <v>36</v>
+      </c>
       <c r="H11" s="12"/>
       <c r="I11" s="13"/>
       <c r="J11" s="14"/>
       <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
+      <c r="L11" s="16"/>
       <c r="M11" s="2" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
carlsberg adding sample templates
</commit_message>
<xml_diff>
--- a/Projects/CARLSBRGHK/Data/Template.xlsx
+++ b/Projects/CARLSBRGHK/Data/Template.xlsx
@@ -116,7 +116,7 @@
     <t xml:space="preserve">manufacturer</t>
   </si>
   <si>
-    <t xml:space="preserve">Diageo</t>
+    <t xml:space="preserve">Carlsberg Brewery Hong Kong Ltd</t>
   </si>
   <si>
     <t xml:space="preserve">store</t>
@@ -417,15 +417,16 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B3 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="105.969387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="104.755102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="7" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -562,25 +563,25 @@
   <dimension ref="1:11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="51.4336734693878"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="60.2040816326531"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="7" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="7" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="7" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="7" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="7" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="7" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="17" min="15" style="7" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="7" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="7" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="52.0102040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="59.3979591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="7" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="7" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="28.7959183673469"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="7" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="7" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="7" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="7" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="17" min="15" style="7" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="7" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="7" width="9.71938775510204"/>
   </cols>
   <sheetData>
     <row r="1" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
update template config with store types
</commit_message>
<xml_diff>
--- a/Projects/CARLSBRGHK/Data/Template.xlsx
+++ b/Projects/CARLSBRGHK/Data/Template.xlsx
@@ -122,7 +122,7 @@
     <t xml:space="preserve">store</t>
   </si>
   <si>
-    <t xml:space="preserve">Off Trade, On Trade</t>
+    <t xml:space="preserve">PNS, WLC, Test</t>
   </si>
   <si>
     <t xml:space="preserve">scene_type</t>
@@ -422,11 +422,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="104.755102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="4" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="103.540816326531"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -562,26 +563,26 @@
   </sheetPr>
   <dimension ref="1:11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="52.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="59.3979591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="7" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="7" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="28.7959183673469"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="7" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="7" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="7" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="7" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="17" min="15" style="7" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="7" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="7" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="51.4336734693878"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="58.719387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="7" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="7" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="7" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="7" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="7" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="7" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="17" min="15" style="7" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="7" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="7" width="9.58673469387755"/>
   </cols>
   <sheetData>
     <row r="1" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
fixing denominator pushing new tests
</commit_message>
<xml_diff>
--- a/Projects/CARLSBRGHK/Data/Template.xlsx
+++ b/Projects/CARLSBRGHK/Data/Template.xlsx
@@ -422,12 +422,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="103.540816326531"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="4" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="102.459183673469"/>
+    <col collapsed="false" hidden="false" max="7" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -564,25 +563,25 @@
   <dimension ref="1:11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="51.4336734693878"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="58.719387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="7" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="7" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="28.484693877551"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="7" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="7" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="7" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="7" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="17" min="15" style="7" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="7" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="7" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="50.7551020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="58.0459183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="7" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="7" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="28.0765306122449"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="7" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="7" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="7" width="6.75"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="7" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="17" min="15" style="7" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="7" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="7" width="9.44897959183673"/>
   </cols>
   <sheetData>
     <row r="1" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6957,7 +6956,7 @@
       <c r="K9" s="15"/>
       <c r="L9" s="16"/>
       <c r="M9" s="2" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="N9" s="2" t="s">
         <v>34</v>
@@ -8003,7 +8002,7 @@
       <c r="K10" s="15"/>
       <c r="L10" s="16"/>
       <c r="M10" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>34</v>

</xml_diff>